<commit_message>
started populating rq5 table
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ5.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E1112EE-0303-4DFC-9D5E-D32BC9F57581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED66319B-95B0-47A6-9260-457F82BAB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Variables</t>
   </si>
@@ -48,6 +48,12 @@
     <t>Scenario</t>
   </si>
   <si>
+    <t>Most aligned target</t>
+  </si>
+  <si>
+    <t>Least aligned target</t>
+  </si>
+  <si>
     <t>Alignment score (Delegator|Most aligned target)</t>
   </si>
   <si>
@@ -63,6 +69,12 @@
     <t>TA2_Name</t>
   </si>
   <si>
+    <t>Alignment score (Delegator|ADM(most))</t>
+  </si>
+  <si>
+    <t>Alignment score (Delegator|ADM(least))</t>
+  </si>
+  <si>
     <t>Match_MostAligned</t>
   </si>
   <si>
@@ -87,6 +99,9 @@
     <t>TA1</t>
   </si>
   <si>
+    <t>TA1 server</t>
+  </si>
+  <si>
     <t>Calculated from probe responses</t>
   </si>
   <si>
@@ -102,7 +117,22 @@
     <t>Scenario presented to the delegators in DM observation materials</t>
   </si>
   <si>
+    <t>Target with the highest alignment score for the delegator on the text scenario</t>
+  </si>
+  <si>
+    <t>Target with the lowest alignment score for the delegator on the text scenario</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the delegator and a target</t>
+  </si>
+  <si>
     <t>Calculated alignment score between the KDMA measurement of a delegator and a group target</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the delegator and the aligned ADM run on the same scenario at the most aligned target</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the delegator and the aligned ADM run on the same scenario at the least aligned target</t>
   </si>
   <si>
     <t>% of exact matches on probe responses between delegator and ADM run on same scenario at most aligned target</t>
@@ -493,19 +523,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="16.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="24" width="16.7109375" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45.75">
+    <row r="1" spans="1:17" ht="45.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,116 +575,146 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="30.75">
+    <row r="2" spans="1:17" ht="30.75">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="121.5">
+    <row r="3" spans="1:17" ht="137.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="126" customHeight="1">
+    <row r="4" spans="1:17" ht="126" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated RQ5 and variables to base off text instead of delegation
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ5.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED66319B-95B0-47A6-9260-457F82BAB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D2B426-8ECA-4613-96A5-0951AE316E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Variables</t>
   </si>
   <si>
-    <t>Delegator_ID</t>
+    <t>Participant_ID</t>
   </si>
   <si>
     <t>TA1_Name</t>
@@ -54,25 +54,25 @@
     <t>Least aligned target</t>
   </si>
   <si>
-    <t>Alignment score (Delegator|Most aligned target)</t>
-  </si>
-  <si>
-    <t>Alignment score (Delegator|Least aligned target)</t>
+    <t>Alignment score (Participant|Most aligned target)</t>
+  </si>
+  <si>
+    <t>Alignment score (Participant|Least aligned target)</t>
   </si>
   <si>
     <t>Group target</t>
   </si>
   <si>
-    <t>Alignment score (Delegator|group target)</t>
+    <t>Alignment score (Participant|group target)</t>
   </si>
   <si>
     <t>TA2_Name</t>
   </si>
   <si>
-    <t>Alignment score (Delegator|ADM(most))</t>
-  </si>
-  <si>
-    <t>Alignment score (Delegator|ADM(least))</t>
+    <t>Alignment score (Participant|ADM(most))</t>
+  </si>
+  <si>
+    <t>Alignment score (Participant|ADM(least))</t>
   </si>
   <si>
     <t>Match_MostAligned</t>
@@ -87,10 +87,10 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Delegation survey response log</t>
-  </si>
-  <si>
-    <t>Delegation survey loading log</t>
+    <t>Text scenario</t>
+  </si>
+  <si>
+    <t>Text scenario loading log</t>
   </si>
   <si>
     <t>TA1 Server</t>
@@ -108,40 +108,43 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>Used to track and identify participants, also called participant ID</t>
+    <t>Used to track and identify participants, also called delegator ID</t>
   </si>
   <si>
     <t>Origin of scenario</t>
   </si>
   <si>
-    <t>Scenario presented to the delegators in DM observation materials</t>
-  </si>
-  <si>
-    <t>Target with the highest alignment score for the delegator on the text scenario</t>
-  </si>
-  <si>
-    <t>Target with the lowest alignment score for the delegator on the text scenario</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the delegator and a target</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of a delegator and a group target</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the delegator and the aligned ADM run on the same scenario at the most aligned target</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the delegator and the aligned ADM run on the same scenario at the least aligned target</t>
-  </si>
-  <si>
-    <t>% of exact matches on probe responses between delegator and ADM run on same scenario at most aligned target</t>
-  </si>
-  <si>
-    <t>% of exact matches on probe responses between delegator and ADM run on same scenario at least aligned target</t>
-  </si>
-  <si>
-    <t>% of exact matches on probe responses between delegator and ADM run on same scenario at group target</t>
+    <t>Scenario presented to the participant in the text scenarios</t>
+  </si>
+  <si>
+    <t>Target with the highest alignment score for the participant on the text scenario</t>
+  </si>
+  <si>
+    <t>Target with the lowest alignment score for the participant on the text scenario</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the participant and a target</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a participant and a group target</t>
+  </si>
+  <si>
+    <t>Source of ADM responses</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the participant and the aligned ADM run on the same scenario at the most aligned target</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the participant and the aligned ADM run on the same scenario at the least aligned target</t>
+  </si>
+  <si>
+    <t>% of exact matches on probe responses between participant and ADM run on same scenario at most aligned target</t>
+  </si>
+  <si>
+    <t>% of exact matches on probe responses between participant and ADM run on same scenario at least aligned target</t>
+  </si>
+  <si>
+    <t>% of exact matches on probe responses among group members and ADM run on same scenario at group target</t>
   </si>
   <si>
     <t>Levels</t>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,10 +599,10 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -615,9 +618,6 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>22</v>
@@ -663,58 +663,61 @@
       <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="126" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>